<commit_message>
new data with new performance unit
</commit_message>
<xml_diff>
--- a/project6/Workbook1.xlsx
+++ b/project6/Workbook1.xlsx
@@ -246,25 +246,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.013</c:v>
+                  <c:v>13.796</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.013</c:v>
+                  <c:v>20.967</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.014</c:v>
+                  <c:v>20.258</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.014</c:v>
+                  <c:v>13.676</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.014</c:v>
+                  <c:v>13.413</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.014</c:v>
+                  <c:v>20.686</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.016</c:v>
+                  <c:v>12.488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,25 +346,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.724</c:v>
+                  <c:v>1182.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.964</c:v>
+                  <c:v>1269.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.112</c:v>
+                  <c:v>994.386</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.733</c:v>
+                  <c:v>1219.479</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.765</c:v>
+                  <c:v>731.6420000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.746</c:v>
+                  <c:v>1118.107</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.733</c:v>
+                  <c:v>725.101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -446,25 +446,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.475</c:v>
+                  <c:v>1716.689</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.493</c:v>
+                  <c:v>2516.29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.421</c:v>
+                  <c:v>1434.176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.475</c:v>
+                  <c:v>2320.51</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.448</c:v>
+                  <c:v>1515.003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.497</c:v>
+                  <c:v>2288.893</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.461</c:v>
+                  <c:v>1448.357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -546,25 +546,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.864</c:v>
+                  <c:v>4193.725</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.429</c:v>
+                  <c:v>4942.29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.884</c:v>
+                  <c:v>2743.197</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.92</c:v>
+                  <c:v>3484.104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.943</c:v>
+                  <c:v>3419.862</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.972</c:v>
+                  <c:v>2516.611</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.932</c:v>
+                  <c:v>3092.812</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -646,25 +646,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7.799</c:v>
+                  <c:v>7213.091</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.701</c:v>
+                  <c:v>6114.948</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.201000000000001</c:v>
+                  <c:v>4728.411</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.233000000000001</c:v>
+                  <c:v>7127.727</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.782</c:v>
+                  <c:v>5521.32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.13</c:v>
+                  <c:v>4736.65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.788</c:v>
+                  <c:v>6568.801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -746,25 +746,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>16.845</c:v>
+                  <c:v>11652.414</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.788</c:v>
+                  <c:v>9467.281999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.33</c:v>
+                  <c:v>12352.483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.966</c:v>
+                  <c:v>13849.421</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.001</c:v>
+                  <c:v>13419.69</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.398</c:v>
+                  <c:v>9700.235</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.562</c:v>
+                  <c:v>11984.257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -781,11 +781,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1842511824"/>
-        <c:axId val="-1842509504"/>
+        <c:axId val="568495776"/>
+        <c:axId val="568497824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1842511824"/>
+        <c:axId val="568495776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1842509504"/>
+        <c:crossAx val="568497824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -836,7 +836,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1842509504"/>
+        <c:axId val="568497824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,7 +886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1842511824"/>
+        <c:crossAx val="568495776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1089,22 +1089,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.013</c:v>
+                  <c:v>13.796</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.724</c:v>
+                  <c:v>1182.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.475</c:v>
+                  <c:v>1716.689</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.864</c:v>
+                  <c:v>4193.725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.799</c:v>
+                  <c:v>7213.091</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.845</c:v>
+                  <c:v>11652.414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,22 +1182,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.013</c:v>
+                  <c:v>20.967</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.964</c:v>
+                  <c:v>1269.41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.493</c:v>
+                  <c:v>2516.29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.429</c:v>
+                  <c:v>4942.29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.701</c:v>
+                  <c:v>6114.948</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.788</c:v>
+                  <c:v>9467.281999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1275,22 +1275,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.014</c:v>
+                  <c:v>20.258</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.112</c:v>
+                  <c:v>994.386</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.421</c:v>
+                  <c:v>1434.176</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.884</c:v>
+                  <c:v>2743.197</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.201000000000001</c:v>
+                  <c:v>4728.411</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.33</c:v>
+                  <c:v>12352.483</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1368,22 +1368,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.014</c:v>
+                  <c:v>13.676</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.733</c:v>
+                  <c:v>1219.479</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.475</c:v>
+                  <c:v>2320.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.92</c:v>
+                  <c:v>3484.104</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.233000000000001</c:v>
+                  <c:v>7127.727</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.966</c:v>
+                  <c:v>13849.421</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1461,22 +1461,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.014</c:v>
+                  <c:v>13.413</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.765</c:v>
+                  <c:v>731.6420000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.448</c:v>
+                  <c:v>1515.003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.943</c:v>
+                  <c:v>3419.862</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.782</c:v>
+                  <c:v>5521.32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.001</c:v>
+                  <c:v>13419.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1554,22 +1554,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.014</c:v>
+                  <c:v>20.686</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.746</c:v>
+                  <c:v>1118.107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.497</c:v>
+                  <c:v>2288.893</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.972</c:v>
+                  <c:v>2516.611</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.13</c:v>
+                  <c:v>4736.65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.398</c:v>
+                  <c:v>9700.235</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1653,22 +1653,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.016</c:v>
+                  <c:v>12.488</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.733</c:v>
+                  <c:v>725.101</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.461</c:v>
+                  <c:v>1448.357</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.932</c:v>
+                  <c:v>3092.812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.788</c:v>
+                  <c:v>6568.801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.562</c:v>
+                  <c:v>11984.257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1685,11 +1685,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1734214304"/>
-        <c:axId val="-1734212528"/>
+        <c:axId val="563594832"/>
+        <c:axId val="563597312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1734214304"/>
+        <c:axId val="563594832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1732,7 +1732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734212528"/>
+        <c:crossAx val="563597312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1740,7 +1740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1734212528"/>
+        <c:axId val="563597312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1790,7 +1790,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734214304"/>
+        <c:crossAx val="563594832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1997,25 +1997,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.014</c:v>
+                  <c:v>17.284</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.013</c:v>
+                  <c:v>16.57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.013</c:v>
+                  <c:v>18.933</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.012</c:v>
+                  <c:v>18.504</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.013</c:v>
+                  <c:v>16.594</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.016</c:v>
+                  <c:v>13.355</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.011</c:v>
+                  <c:v>12.901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2097,25 +2097,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.73</c:v>
+                  <c:v>1245.748</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.763</c:v>
+                  <c:v>723.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.73</c:v>
+                  <c:v>1042.739</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.704</c:v>
+                  <c:v>1265.333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.7</c:v>
+                  <c:v>863.966</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.749</c:v>
+                  <c:v>1006.203</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.737</c:v>
+                  <c:v>897.9349999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2197,25 +2197,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.481</c:v>
+                  <c:v>1471.805</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.485</c:v>
+                  <c:v>1887.367</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.486</c:v>
+                  <c:v>2069.397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.493</c:v>
+                  <c:v>1940.981</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.477</c:v>
+                  <c:v>2168.294</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.898</c:v>
+                  <c:v>1788.921</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.492</c:v>
+                  <c:v>2385.285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2297,25 +2297,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.62</c:v>
+                  <c:v>2892.217</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.482</c:v>
+                  <c:v>4359.349</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.154</c:v>
+                  <c:v>3064.457</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.002</c:v>
+                  <c:v>4940.194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.412</c:v>
+                  <c:v>3192.945</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.069</c:v>
+                  <c:v>4288.269</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.329</c:v>
+                  <c:v>3854.598</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2397,25 +2397,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.931</c:v>
+                  <c:v>4771.471</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.161</c:v>
+                  <c:v>5217.945</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.108000000000001</c:v>
+                  <c:v>5094.694</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.97</c:v>
+                  <c:v>5162.239</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.178000000000001</c:v>
+                  <c:v>5323.639</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.239000000000001</c:v>
+                  <c:v>5184.624</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.818</c:v>
+                  <c:v>7212.185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2497,25 +2497,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>14.819</c:v>
+                  <c:v>10259.801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.458</c:v>
+                  <c:v>10002.001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.656</c:v>
+                  <c:v>9275.523999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.115</c:v>
+                  <c:v>8909.114</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.292</c:v>
+                  <c:v>9204.333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.713</c:v>
+                  <c:v>9324.477999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.012</c:v>
+                  <c:v>8906.049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2532,11 +2532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1734296096"/>
-        <c:axId val="-1733406784"/>
+        <c:axId val="563636928"/>
+        <c:axId val="563639408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1734296096"/>
+        <c:axId val="563636928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2579,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1733406784"/>
+        <c:crossAx val="563639408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2587,7 +2587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1733406784"/>
+        <c:axId val="563639408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2637,7 +2637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1734296096"/>
+        <c:crossAx val="563636928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2840,22 +2840,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.014</c:v>
+                  <c:v>17.284</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73</c:v>
+                  <c:v>1245.748</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.481</c:v>
+                  <c:v>1471.805</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.62</c:v>
+                  <c:v>2892.217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.931</c:v>
+                  <c:v>4771.471</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.819</c:v>
+                  <c:v>10259.801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2933,22 +2933,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.013</c:v>
+                  <c:v>16.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.763</c:v>
+                  <c:v>723.47</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.485</c:v>
+                  <c:v>1887.367</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.482</c:v>
+                  <c:v>4359.349</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.161</c:v>
+                  <c:v>5217.945</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.458</c:v>
+                  <c:v>10002.001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3026,22 +3026,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.013</c:v>
+                  <c:v>18.933</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73</c:v>
+                  <c:v>1042.739</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.486</c:v>
+                  <c:v>2069.397</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.154</c:v>
+                  <c:v>3064.457</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.108000000000001</c:v>
+                  <c:v>5094.694</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.656</c:v>
+                  <c:v>9275.523999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3119,22 +3119,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.012</c:v>
+                  <c:v>18.504</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.704</c:v>
+                  <c:v>1265.333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.493</c:v>
+                  <c:v>1940.981</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.002</c:v>
+                  <c:v>4940.194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.97</c:v>
+                  <c:v>5162.239</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.115</c:v>
+                  <c:v>8909.114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3212,22 +3212,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.013</c:v>
+                  <c:v>16.594</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7</c:v>
+                  <c:v>863.966</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.477</c:v>
+                  <c:v>2168.294</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.412</c:v>
+                  <c:v>3192.945</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.178000000000001</c:v>
+                  <c:v>5323.639</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.292</c:v>
+                  <c:v>9204.333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3305,22 +3305,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.016</c:v>
+                  <c:v>13.355</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.749</c:v>
+                  <c:v>1006.203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.898</c:v>
+                  <c:v>1788.921</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.069</c:v>
+                  <c:v>4288.269</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.239000000000001</c:v>
+                  <c:v>5184.624</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.713</c:v>
+                  <c:v>9324.477999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3404,22 +3404,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.011</c:v>
+                  <c:v>12.901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.737</c:v>
+                  <c:v>897.9349999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.492</c:v>
+                  <c:v>2385.285</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.329</c:v>
+                  <c:v>3854.598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.818</c:v>
+                  <c:v>7212.185</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.012</c:v>
+                  <c:v>8906.049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3436,11 +3436,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1733048048"/>
-        <c:axId val="-1730988976"/>
+        <c:axId val="563682432"/>
+        <c:axId val="563684912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1733048048"/>
+        <c:axId val="563682432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3483,7 +3483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1730988976"/>
+        <c:crossAx val="563684912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3491,7 +3491,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1730988976"/>
+        <c:axId val="563684912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3541,7 +3541,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1733048048"/>
+        <c:crossAx val="563682432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6185,7 +6185,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:G20"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6215,22 +6215,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.2999999999999999E-2</v>
+        <v>13.795999999999999</v>
       </c>
       <c r="C2">
-        <v>0.72399999999999998</v>
+        <v>1182</v>
       </c>
       <c r="D2">
-        <v>1.4750000000000001</v>
+        <v>1716.6890000000001</v>
       </c>
       <c r="E2">
-        <v>2.8639999999999999</v>
+        <v>4193.7250000000004</v>
       </c>
       <c r="F2">
-        <v>7.7990000000000004</v>
+        <v>7213.0910000000003</v>
       </c>
       <c r="G2">
-        <v>16.844999999999999</v>
+        <v>11652.414000000001</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -6238,22 +6238,22 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1.2999999999999999E-2</v>
+        <v>20.966999999999999</v>
       </c>
       <c r="C3">
-        <v>0.96399999999999997</v>
+        <v>1269.4100000000001</v>
       </c>
       <c r="D3">
-        <v>1.4930000000000001</v>
+        <v>2516.29</v>
       </c>
       <c r="E3">
-        <v>2.4289999999999998</v>
+        <v>4942.29</v>
       </c>
       <c r="F3">
-        <v>7.7009999999999996</v>
+        <v>6114.9480000000003</v>
       </c>
       <c r="G3">
-        <v>16.788</v>
+        <v>9467.2819999999992</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -6261,22 +6261,22 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>1.4E-2</v>
+        <v>20.257999999999999</v>
       </c>
       <c r="C4">
-        <v>1.1120000000000001</v>
+        <v>994.38599999999997</v>
       </c>
       <c r="D4">
-        <v>1.421</v>
+        <v>1434.1759999999999</v>
       </c>
       <c r="E4">
-        <v>2.8839999999999999</v>
+        <v>2743.1970000000001</v>
       </c>
       <c r="F4">
-        <v>8.2010000000000005</v>
+        <v>4728.4110000000001</v>
       </c>
       <c r="G4">
-        <v>17.329999999999998</v>
+        <v>12352.483</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -6284,22 +6284,22 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>1.4E-2</v>
+        <v>13.676</v>
       </c>
       <c r="C5">
-        <v>0.73299999999999998</v>
+        <v>1219.479</v>
       </c>
       <c r="D5">
-        <v>1.4750000000000001</v>
+        <v>2320.5100000000002</v>
       </c>
       <c r="E5">
-        <v>2.92</v>
+        <v>3484.1039999999998</v>
       </c>
       <c r="F5">
-        <v>8.2330000000000005</v>
+        <v>7127.7269999999999</v>
       </c>
       <c r="G5">
-        <v>16.966000000000001</v>
+        <v>13849.421</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -6307,22 +6307,22 @@
         <v>128</v>
       </c>
       <c r="B6">
-        <v>1.4E-2</v>
+        <v>13.413</v>
       </c>
       <c r="C6">
-        <v>0.76500000000000001</v>
+        <v>731.64200000000005</v>
       </c>
       <c r="D6">
-        <v>1.448</v>
+        <v>1515.0029999999999</v>
       </c>
       <c r="E6">
-        <v>2.9430000000000001</v>
+        <v>3419.8620000000001</v>
       </c>
       <c r="F6">
-        <v>8.782</v>
+        <v>5521.32</v>
       </c>
       <c r="G6">
-        <v>17.001000000000001</v>
+        <v>13419.69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -6330,22 +6330,22 @@
         <v>512</v>
       </c>
       <c r="B7">
-        <v>1.4E-2</v>
+        <v>20.686</v>
       </c>
       <c r="C7">
-        <v>0.746</v>
+        <v>1118.107</v>
       </c>
       <c r="D7">
-        <v>1.4970000000000001</v>
+        <v>2288.893</v>
       </c>
       <c r="E7">
-        <v>2.972</v>
+        <v>2516.6109999999999</v>
       </c>
       <c r="F7">
-        <v>7.13</v>
+        <v>4736.6499999999996</v>
       </c>
       <c r="G7">
-        <v>16.398</v>
+        <v>9700.2350000000006</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -6353,22 +6353,22 @@
         <v>1024</v>
       </c>
       <c r="B8">
-        <v>1.6E-2</v>
+        <v>12.488</v>
       </c>
       <c r="C8">
-        <v>0.73299999999999998</v>
+        <v>725.101</v>
       </c>
       <c r="D8">
-        <v>1.4610000000000001</v>
+        <v>1448.357</v>
       </c>
       <c r="E8">
-        <v>2.9319999999999999</v>
+        <v>3092.8119999999999</v>
       </c>
       <c r="F8">
-        <v>8.7880000000000003</v>
+        <v>6568.8010000000004</v>
       </c>
       <c r="G8">
-        <v>13.561999999999999</v>
+        <v>11984.257</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -6396,22 +6396,22 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>1.4E-2</v>
+        <v>17.283999999999999</v>
       </c>
       <c r="C14">
-        <v>0.73</v>
+        <v>1245.748</v>
       </c>
       <c r="D14">
-        <v>1.4810000000000001</v>
+        <v>1471.8050000000001</v>
       </c>
       <c r="E14">
-        <v>2.62</v>
+        <v>2892.2170000000001</v>
       </c>
       <c r="F14">
-        <v>6.931</v>
+        <v>4771.4709999999995</v>
       </c>
       <c r="G14">
-        <v>14.819000000000001</v>
+        <v>10259.800999999999</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -6419,22 +6419,22 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>1.2999999999999999E-2</v>
+        <v>16.57</v>
       </c>
       <c r="C15">
-        <v>0.76300000000000001</v>
+        <v>723.47</v>
       </c>
       <c r="D15">
-        <v>1.4850000000000001</v>
+        <v>1887.367</v>
       </c>
       <c r="E15">
-        <v>2.4820000000000002</v>
+        <v>4359.3490000000002</v>
       </c>
       <c r="F15">
-        <v>8.1609999999999996</v>
+        <v>5217.9449999999997</v>
       </c>
       <c r="G15">
-        <v>14.458</v>
+        <v>10002.001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -6442,22 +6442,22 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>1.2999999999999999E-2</v>
+        <v>18.933</v>
       </c>
       <c r="C16">
-        <v>0.73</v>
+        <v>1042.739</v>
       </c>
       <c r="D16">
-        <v>1.486</v>
+        <v>2069.3969999999999</v>
       </c>
       <c r="E16">
-        <v>2.1539999999999999</v>
+        <v>3064.4569999999999</v>
       </c>
       <c r="F16">
-        <v>8.1080000000000005</v>
+        <v>5094.6940000000004</v>
       </c>
       <c r="G16">
-        <v>14.656000000000001</v>
+        <v>9275.5239999999994</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -6465,22 +6465,22 @@
         <v>32</v>
       </c>
       <c r="B17">
-        <v>1.2E-2</v>
+        <v>18.504000000000001</v>
       </c>
       <c r="C17">
-        <v>0.70399999999999996</v>
+        <v>1265.3330000000001</v>
       </c>
       <c r="D17">
-        <v>1.4930000000000001</v>
+        <v>1940.981</v>
       </c>
       <c r="E17">
-        <v>2.0019999999999998</v>
+        <v>4940.1940000000004</v>
       </c>
       <c r="F17">
-        <v>7.97</v>
+        <v>5162.2389999999996</v>
       </c>
       <c r="G17">
-        <v>16.114999999999998</v>
+        <v>8909.1139999999996</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -6488,22 +6488,22 @@
         <v>128</v>
       </c>
       <c r="B18">
-        <v>1.2999999999999999E-2</v>
+        <v>16.594000000000001</v>
       </c>
       <c r="C18">
-        <v>0.7</v>
+        <v>863.96600000000001</v>
       </c>
       <c r="D18">
-        <v>1.4770000000000001</v>
+        <v>2168.2939999999999</v>
       </c>
       <c r="E18">
-        <v>2.4119999999999999</v>
+        <v>3192.9450000000002</v>
       </c>
       <c r="F18">
-        <v>8.1780000000000008</v>
+        <v>5323.6390000000001</v>
       </c>
       <c r="G18">
-        <v>14.292</v>
+        <v>9204.3330000000005</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -6511,22 +6511,22 @@
         <v>512</v>
       </c>
       <c r="B19">
-        <v>1.6E-2</v>
+        <v>13.355</v>
       </c>
       <c r="C19">
-        <v>0.749</v>
+        <v>1006.203</v>
       </c>
       <c r="D19">
-        <v>1.8979999999999999</v>
+        <v>1788.921</v>
       </c>
       <c r="E19">
-        <v>2.069</v>
+        <v>4288.2690000000002</v>
       </c>
       <c r="F19">
-        <v>8.2390000000000008</v>
+        <v>5184.6239999999998</v>
       </c>
       <c r="G19">
-        <v>14.712999999999999</v>
+        <v>9324.4779999999992</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -6534,22 +6534,22 @@
         <v>1024</v>
       </c>
       <c r="B20">
-        <v>1.0999999999999999E-2</v>
+        <v>12.901</v>
       </c>
       <c r="C20">
-        <v>0.73699999999999999</v>
+        <v>897.93499999999995</v>
       </c>
       <c r="D20">
-        <v>1.492</v>
+        <v>2385.2849999999999</v>
       </c>
       <c r="E20">
-        <v>2.3290000000000002</v>
+        <v>3854.598</v>
       </c>
       <c r="F20">
-        <v>7.8179999999999996</v>
+        <v>7212.1850000000004</v>
       </c>
       <c r="G20">
-        <v>15.012</v>
+        <v>8906.0490000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data q1, fix output bug
</commit_message>
<xml_diff>
--- a/project6/Workbook1.xlsx
+++ b/project6/Workbook1.xlsx
@@ -258,25 +258,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12.937</c:v>
+                  <c:v>12.634</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.942</c:v>
+                  <c:v>12.157</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.311</c:v>
+                  <c:v>9.381</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.746</c:v>
+                  <c:v>17.012</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.681</c:v>
+                  <c:v>12.836</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.857</c:v>
+                  <c:v>15.245</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.472</c:v>
+                  <c:v>16.843</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,25 +358,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>36.989</c:v>
+                  <c:v>297.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>403.054</c:v>
+                  <c:v>730.2670000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.288</c:v>
+                  <c:v>1044.486</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.625</c:v>
+                  <c:v>1382.496</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>885.9160000000001</c:v>
+                  <c:v>1492.512</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>421.161</c:v>
+                  <c:v>1423.752</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>571.46</c:v>
+                  <c:v>1183.366</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -458,25 +458,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>189.549</c:v>
+                  <c:v>335.415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93.55</c:v>
+                  <c:v>1028.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>599.921</c:v>
+                  <c:v>1924.526</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>549.504</c:v>
+                  <c:v>2127.235</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1800.294</c:v>
+                  <c:v>2248.31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>136.902</c:v>
+                  <c:v>2774.568</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1941.541</c:v>
+                  <c:v>2697.739</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,25 +558,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>341.48</c:v>
+                  <c:v>347.764</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550.849</c:v>
+                  <c:v>1199.128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2059.355</c:v>
+                  <c:v>2953.169</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1011.505</c:v>
+                  <c:v>3769.023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2274.756</c:v>
+                  <c:v>4528.479</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3702.664</c:v>
+                  <c:v>4477.334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2674.969</c:v>
+                  <c:v>4477.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -658,25 +658,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>356.207</c:v>
+                  <c:v>357.583</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1188.902</c:v>
+                  <c:v>1304.054</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3181.765</c:v>
+                  <c:v>3558.433</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3544.414</c:v>
+                  <c:v>5131.112</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4368.411</c:v>
+                  <c:v>6110.645</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>298.109</c:v>
+                  <c:v>6356.547</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4835.685</c:v>
+                  <c:v>6149.519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -758,25 +758,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>361.557</c:v>
+                  <c:v>368.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1323.079</c:v>
+                  <c:v>1405.909</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65.479</c:v>
+                  <c:v>4658.192</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6328.866</c:v>
+                  <c:v>6913.257</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2810.842</c:v>
+                  <c:v>8814.017</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2355.059</c:v>
+                  <c:v>9918.18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>81.784</c:v>
+                  <c:v>9732.953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -793,11 +793,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1918472064"/>
-        <c:axId val="-1918470000"/>
+        <c:axId val="1313131648"/>
+        <c:axId val="1313133008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1918472064"/>
+        <c:axId val="1313131648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1918470000"/>
+        <c:crossAx val="1313133008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -848,7 +848,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1918470000"/>
+        <c:axId val="1313133008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1918472064"/>
+        <c:crossAx val="1313131648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1101,22 +1101,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>12.937</c:v>
+                  <c:v>12.634</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.989</c:v>
+                  <c:v>297.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>189.549</c:v>
+                  <c:v>335.415</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>341.48</c:v>
+                  <c:v>347.764</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>356.207</c:v>
+                  <c:v>357.583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>361.557</c:v>
+                  <c:v>368.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1194,22 +1194,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>12.942</c:v>
+                  <c:v>12.157</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>403.054</c:v>
+                  <c:v>730.2670000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>93.55</c:v>
+                  <c:v>1028.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>550.849</c:v>
+                  <c:v>1199.128</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1188.902</c:v>
+                  <c:v>1304.054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1323.079</c:v>
+                  <c:v>1405.909</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,22 +1287,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>11.311</c:v>
+                  <c:v>9.381</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51.288</c:v>
+                  <c:v>1044.486</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>599.921</c:v>
+                  <c:v>1924.526</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2059.355</c:v>
+                  <c:v>2953.169</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3181.765</c:v>
+                  <c:v>3558.433</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>65.479</c:v>
+                  <c:v>4658.192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1380,22 +1380,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>12.746</c:v>
+                  <c:v>17.012</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.625</c:v>
+                  <c:v>1382.496</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>549.504</c:v>
+                  <c:v>2127.235</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1011.505</c:v>
+                  <c:v>3769.023</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3544.414</c:v>
+                  <c:v>5131.112</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6328.866</c:v>
+                  <c:v>6913.257</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1473,22 +1473,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>14.681</c:v>
+                  <c:v>12.836</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>885.9160000000001</c:v>
+                  <c:v>1492.512</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1800.294</c:v>
+                  <c:v>2248.31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2274.756</c:v>
+                  <c:v>4528.479</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4368.411</c:v>
+                  <c:v>6110.645</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2810.842</c:v>
+                  <c:v>8814.017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1566,22 +1566,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.857</c:v>
+                  <c:v>15.245</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>421.161</c:v>
+                  <c:v>1423.752</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136.902</c:v>
+                  <c:v>2774.568</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3702.664</c:v>
+                  <c:v>4477.334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>298.109</c:v>
+                  <c:v>6356.547</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2355.059</c:v>
+                  <c:v>9918.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1665,22 +1665,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>15.472</c:v>
+                  <c:v>16.843</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>571.46</c:v>
+                  <c:v>1183.366</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1941.541</c:v>
+                  <c:v>2697.739</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2674.969</c:v>
+                  <c:v>4477.87</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4835.685</c:v>
+                  <c:v>6149.519</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81.784</c:v>
+                  <c:v>9732.953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1697,11 +1697,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1967969728"/>
-        <c:axId val="-1967967248"/>
+        <c:axId val="1313161088"/>
+        <c:axId val="1313162880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1967969728"/>
+        <c:axId val="1313161088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +1744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1967967248"/>
+        <c:crossAx val="1313162880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1752,7 +1752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1967967248"/>
+        <c:axId val="1313162880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1802,7 +1802,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1967969728"/>
+        <c:crossAx val="1313161088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2544,11 +2544,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1967922448"/>
-        <c:axId val="-1967919968"/>
+        <c:axId val="1313208048"/>
+        <c:axId val="1313210528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1967922448"/>
+        <c:axId val="1313208048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2591,7 +2591,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1967919968"/>
+        <c:crossAx val="1313210528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2599,7 +2599,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1967919968"/>
+        <c:axId val="1313210528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2649,7 +2649,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1967922448"/>
+        <c:crossAx val="1313208048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3448,11 +3448,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1918428912"/>
-        <c:axId val="-1918426432"/>
+        <c:axId val="1313253504"/>
+        <c:axId val="1313255984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1918428912"/>
+        <c:axId val="1313253504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3495,7 +3495,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1918426432"/>
+        <c:crossAx val="1313255984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3503,7 +3503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1918426432"/>
+        <c:axId val="1313255984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3553,7 +3553,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1918428912"/>
+        <c:crossAx val="1313253504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3865,11 +3865,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1918396320"/>
-        <c:axId val="-1918392272"/>
+        <c:axId val="1313263312"/>
+        <c:axId val="1313267360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1918396320"/>
+        <c:axId val="1313263312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4007,12 +4007,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1918392272"/>
+        <c:crossAx val="1313267360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1918392272"/>
+        <c:axId val="1313267360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4165,7 +4165,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1918396320"/>
+        <c:crossAx val="1313263312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7363,7 +7363,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7393,22 +7393,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>12.936999999999999</v>
+        <v>12.634</v>
       </c>
       <c r="C2">
-        <v>36.988999999999997</v>
+        <v>297.75</v>
       </c>
       <c r="D2">
-        <v>189.54900000000001</v>
+        <v>335.41500000000002</v>
       </c>
       <c r="E2">
-        <v>341.48</v>
+        <v>347.76400000000001</v>
       </c>
       <c r="F2">
-        <v>356.20699999999999</v>
+        <v>357.58300000000003</v>
       </c>
       <c r="G2">
-        <v>361.55700000000002</v>
+        <v>368.02</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -7416,22 +7416,22 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>12.942</v>
+        <v>12.157</v>
       </c>
       <c r="C3">
-        <v>403.05399999999997</v>
+        <v>730.26700000000005</v>
       </c>
       <c r="D3">
-        <v>93.55</v>
+        <v>1028.4000000000001</v>
       </c>
       <c r="E3">
-        <v>550.84900000000005</v>
+        <v>1199.1279999999999</v>
       </c>
       <c r="F3">
-        <v>1188.902</v>
+        <v>1304.0540000000001</v>
       </c>
       <c r="G3">
-        <v>1323.079</v>
+        <v>1405.9090000000001</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -7439,22 +7439,22 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>11.311</v>
+        <v>9.3810000000000002</v>
       </c>
       <c r="C4">
-        <v>51.287999999999997</v>
+        <v>1044.4860000000001</v>
       </c>
       <c r="D4">
-        <v>599.92100000000005</v>
+        <v>1924.5260000000001</v>
       </c>
       <c r="E4">
-        <v>2059.355</v>
+        <v>2953.1689999999999</v>
       </c>
       <c r="F4">
-        <v>3181.7649999999999</v>
+        <v>3558.433</v>
       </c>
       <c r="G4">
-        <v>65.478999999999999</v>
+        <v>4658.192</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7462,22 +7462,22 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>12.746</v>
+        <v>17.012</v>
       </c>
       <c r="C5">
-        <v>3.625</v>
+        <v>1382.4960000000001</v>
       </c>
       <c r="D5">
-        <v>549.50400000000002</v>
+        <v>2127.2350000000001</v>
       </c>
       <c r="E5">
-        <v>1011.505</v>
+        <v>3769.0230000000001</v>
       </c>
       <c r="F5">
-        <v>3544.4140000000002</v>
+        <v>5131.1120000000001</v>
       </c>
       <c r="G5">
-        <v>6328.866</v>
+        <v>6913.2569999999996</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7485,22 +7485,22 @@
         <v>128</v>
       </c>
       <c r="B6">
-        <v>14.680999999999999</v>
+        <v>12.836</v>
       </c>
       <c r="C6">
-        <v>885.91600000000005</v>
+        <v>1492.5119999999999</v>
       </c>
       <c r="D6">
-        <v>1800.2940000000001</v>
+        <v>2248.31</v>
       </c>
       <c r="E6">
-        <v>2274.7559999999999</v>
+        <v>4528.4790000000003</v>
       </c>
       <c r="F6">
-        <v>4368.4110000000001</v>
+        <v>6110.6450000000004</v>
       </c>
       <c r="G6">
-        <v>2810.8420000000001</v>
+        <v>8814.0169999999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7508,22 +7508,22 @@
         <v>512</v>
       </c>
       <c r="B7">
-        <v>9.8569999999999993</v>
+        <v>15.244999999999999</v>
       </c>
       <c r="C7">
-        <v>421.161</v>
+        <v>1423.752</v>
       </c>
       <c r="D7">
-        <v>136.90199999999999</v>
+        <v>2774.5680000000002</v>
       </c>
       <c r="E7">
-        <v>3702.6640000000002</v>
+        <v>4477.3339999999998</v>
       </c>
       <c r="F7">
-        <v>298.10899999999998</v>
+        <v>6356.5469999999996</v>
       </c>
       <c r="G7">
-        <v>2355.0590000000002</v>
+        <v>9918.18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7531,22 +7531,22 @@
         <v>1024</v>
       </c>
       <c r="B8">
-        <v>15.472</v>
+        <v>16.843</v>
       </c>
       <c r="C8">
-        <v>571.46</v>
+        <v>1183.366</v>
       </c>
       <c r="D8">
-        <v>1941.5409999999999</v>
+        <v>2697.739</v>
       </c>
       <c r="E8">
-        <v>2674.9690000000001</v>
+        <v>4477.87</v>
       </c>
       <c r="F8">
-        <v>4835.6850000000004</v>
+        <v>6149.5190000000002</v>
       </c>
       <c r="G8">
-        <v>81.784000000000006</v>
+        <v>9732.9529999999995</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>